<commit_message>
Create contact scenario for limited user
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="1000" windowWidth="15000" windowHeight="10000"/>
+    <workbookView xWindow="1000" yWindow="1000" windowWidth="15000" windowHeight="10000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CreateNewLead" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateNewContact" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>LeadSource</t>
   </si>
@@ -390,11 +391,11 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="$E$1" sqref="$A$1:$E$1"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="$A$1" sqref="$A$1:$B$2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="9.453125" customWidth="1"/>
     <col min="2" max="2" width="9.1796875" customWidth="1"/>
@@ -442,4 +443,46 @@
   <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection activeCell="$C$5" sqref="$C$5:$C$5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection/>
+  <printOptions/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated for Rapise 7.4
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,14 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Inflectra\InflectraGitProjects\rapise-demo\Salesforce\SfdcFramework\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF0F7C0-30B0-4382-B66A-350E9AA7EC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="1000" windowWidth="15000" windowHeight="10000" activeTab="1"/>
+    <workbookView xWindow="5736" yWindow="1272" windowWidth="24300" windowHeight="15408" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateNewLead" sheetId="1" r:id="rId1"/>
-    <sheet name="CreateNewContact" sheetId="2" r:id="rId2"/>
+    <sheet name="CreateNewContact" sheetId="4" r:id="rId2"/>
+    <sheet name="CreateOpportunity" sheetId="2" r:id="rId3"/>
+    <sheet name="Template" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -17,60 +25,69 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
+    <t>LeadSource</t>
+  </si>
+  <si>
+    <t>Banking</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Contoso</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
     <t>John Smith</t>
   </si>
-  <si>
-    <t>LeadSource</t>
-  </si>
-  <si>
-    <t>FullName</t>
-  </si>
-  <si>
-    <t>Banking</t>
-  </si>
-  <si>
-    <t>John</t>
-  </si>
-  <si>
-    <t>Contoso</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Web</t>
-  </si>
-  <si>
-    <t>Industry</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -83,7 +100,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border outline="0">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -97,13 +114,21 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -391,111 +416,131 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="$A$1" sqref="$A$1:$B$2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.453125" customWidth="1"/>
-    <col min="2" max="2" width="9.1796875" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" customWidth="1"/>
-    <col min="5" max="16384" width="8.7265625"/>
+    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E2" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15524285-D997-456C-9ECB-C45DD772EADF}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="$C$3" sqref="$C$3:$C$3"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection/>
-  <printOptions/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>